<commit_message>
Ratchet White Box and HUD image
</commit_message>
<xml_diff>
--- a/Asset List.xlsx
+++ b/Asset List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kand8\Documents\School 19-20\Game Essentials\2221Fall2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10847775\Documents\Game Essentials\2221Fall2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3F0E45-D4E7-4E70-8F26-7E7BD6BBC237}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,8 +367,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,8 +413,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +462,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -486,12 +497,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -509,10 +521,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -824,27 +838,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" style="14" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
-    <col min="6" max="7" width="9.5546875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="4.77734375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="27.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>86</v>
       </c>
@@ -876,17 +890,17 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -898,17 +912,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="16"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="G6" s="14" t="s">
         <v>96</v>
       </c>
@@ -916,7 +930,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -934,7 +948,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -952,7 +966,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -972,7 +986,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -992,7 +1006,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1003,7 +1017,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1011,13 +1025,13 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1025,7 +1039,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1033,7 +1047,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1055,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1063,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -1057,7 +1071,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1065,7 +1079,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1073,7 +1087,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -1085,7 +1099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
@@ -1099,7 +1113,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1113,7 +1127,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
@@ -1127,7 +1141,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1145,7 +1159,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>23</v>
       </c>
@@ -1163,7 +1177,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>24</v>
       </c>
@@ -1181,7 +1195,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>25</v>
       </c>
@@ -1199,7 +1213,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>26</v>
       </c>
@@ -1217,7 +1231,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
@@ -1235,11 +1249,11 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="16"/>
+      <c r="B31" s="15"/>
       <c r="C31" t="s">
         <v>96</v>
       </c>
@@ -1253,7 +1267,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
@@ -1271,7 +1285,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>30</v>
       </c>
@@ -1289,7 +1303,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
@@ -1304,7 +1318,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>32</v>
       </c>
@@ -1321,11 +1335,11 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="16"/>
+      <c r="B36" s="15"/>
       <c r="C36" t="s">
         <v>96</v>
       </c>
@@ -1339,15 +1353,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
@@ -1365,7 +1379,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>38</v>
       </c>
@@ -1383,7 +1397,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -1401,7 +1415,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>39</v>
       </c>
@@ -1421,7 +1435,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>33</v>
       </c>
@@ -1438,7 +1452,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>34</v>
       </c>
@@ -1455,7 +1469,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
@@ -1473,7 +1487,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>42</v>
       </c>
@@ -1491,7 +1505,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
@@ -1509,7 +1523,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>44</v>
       </c>
@@ -1527,7 +1541,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
@@ -1545,12 +1559,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
@@ -1568,7 +1582,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>47</v>
       </c>
@@ -1586,7 +1600,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>48</v>
       </c>
@@ -1604,11 +1618,11 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="16"/>
+      <c r="B55" s="15"/>
       <c r="C55" t="s">
         <v>96</v>
       </c>
@@ -1622,7 +1636,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>51</v>
       </c>
@@ -1640,7 +1654,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>52</v>
       </c>
@@ -1658,7 +1672,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -1678,18 +1692,18 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B61" s="15"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>55</v>
       </c>
@@ -1698,7 +1712,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>56</v>
       </c>
@@ -1710,17 +1724,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>58</v>
       </c>
@@ -1740,7 +1754,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>59</v>
       </c>
@@ -1758,7 +1772,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>60</v>
       </c>
@@ -1778,7 +1792,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>61</v>
       </c>
@@ -1798,7 +1812,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>62</v>
       </c>
@@ -1818,7 +1832,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>63</v>
       </c>
@@ -1838,7 +1852,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>64</v>
       </c>
@@ -1858,22 +1872,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E74" s="14"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E75" s="14"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E76" s="14"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>67</v>
       </c>
@@ -1893,7 +1907,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>66</v>
       </c>
@@ -1913,7 +1927,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>68</v>
       </c>
@@ -1933,7 +1947,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>69</v>
       </c>
@@ -1953,7 +1967,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>70</v>
       </c>
@@ -1973,7 +1987,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>71</v>
       </c>
@@ -1993,16 +2007,16 @@
         <v>96</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E83" s="14"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>72</v>
       </c>
       <c r="E84" s="14"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>73</v>
       </c>
@@ -2025,7 +2039,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>103</v>
       </c>
@@ -2048,7 +2062,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>104</v>
       </c>
@@ -2071,7 +2085,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>74</v>
       </c>
@@ -2094,7 +2108,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>75</v>
       </c>
@@ -2115,7 +2129,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>76</v>
       </c>
@@ -2138,16 +2152,16 @@
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E91" s="14"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>77</v>
       </c>
       <c r="E92" s="14"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>78</v>
       </c>
@@ -2164,7 +2178,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>105</v>
       </c>
@@ -2181,7 +2195,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>79</v>
       </c>
@@ -2198,16 +2212,16 @@
         <v>96</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E96" s="14"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>80</v>
       </c>
       <c r="E97" s="14"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>81</v>
       </c>
@@ -2224,7 +2238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>82</v>
       </c>
@@ -2241,7 +2255,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>65</v>
       </c>
@@ -2258,7 +2272,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>83</v>
       </c>
@@ -2275,16 +2289,16 @@
         <v>96</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E102" s="14"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>84</v>
       </c>
       <c r="E103" s="14"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>85</v>
       </c>
@@ -2304,16 +2318,16 @@
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B107" s="16"/>
+      <c r="B107" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
File Cleanup and HUD edit
Spread Sheet, File Cleanup, HUD coloring
</commit_message>
<xml_diff>
--- a/Asset List.xlsx
+++ b/Asset List.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="106">
   <si>
     <t>ForeGround:</t>
   </si>
@@ -368,7 +368,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,20 +408,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,11 +452,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
@@ -497,13 +485,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -520,13 +507,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -842,7 +827,7 @@
   <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +889,8 @@
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
       <c r="G4" s="14" t="s">
         <v>96</v>
       </c>
@@ -916,13 +902,17 @@
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="15"/>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
       <c r="G6" s="14" t="s">
         <v>96</v>
       </c>
@@ -1013,6 +1003,9 @@
       <c r="B11" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
       <c r="F11" s="14" t="s">
         <v>96</v>
       </c>
@@ -1024,12 +1017,14 @@
       <c r="B12" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1038,6 +1033,7 @@
       <c r="B14" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -1046,6 +1042,7 @@
       <c r="B15" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1054,6 +1051,7 @@
       <c r="B16" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -1062,6 +1060,7 @@
       <c r="B17" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1070,6 +1069,7 @@
       <c r="B18" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -1078,6 +1078,7 @@
       <c r="B19" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1086,12 +1087,14 @@
       <c r="B20" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="G21" s="14" t="s">
         <v>96</v>
       </c>
@@ -1106,6 +1109,7 @@
       <c r="B22" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C22" s="16"/>
       <c r="G22" s="14" t="s">
         <v>96</v>
       </c>
@@ -1120,6 +1124,7 @@
       <c r="B23" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C23" s="16"/>
       <c r="G23" s="14" t="s">
         <v>96</v>
       </c>
@@ -1134,6 +1139,7 @@
       <c r="B24" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="C24" s="16"/>
       <c r="G24" s="14" t="s">
         <v>96</v>
       </c>
@@ -2328,6 +2334,7 @@
         <v>101</v>
       </c>
       <c r="B107" s="15"/>
+      <c r="C107" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fires and Sparks WB VFX
</commit_message>
<xml_diff>
--- a/Asset List.xlsx
+++ b/Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kand8\Documents\School 19-20\Game Essentials\2221Fall2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438EB132-BF81-4656-AC7D-D90EC8DD1EC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A5843-F4CF-4176-A7AE-9EE263EEFD82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="116">
   <si>
     <t>ForeGround:</t>
   </si>
@@ -382,12 +382,24 @@
   <si>
     <t>VS VFX</t>
   </si>
+  <si>
+    <t>Prototype it</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Mixamo</t>
+  </si>
+  <si>
+    <t>Needs Edit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +450,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Webdings"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Webdings"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -522,7 +548,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -540,8 +566,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -861,13 +890,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="14" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="14" customWidth="1"/>
@@ -948,8 +977,12 @@
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="D4" s="14" t="s">
         <v>96</v>
       </c>
@@ -970,8 +1003,12 @@
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="18"/>
+      <c r="B5" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="D5" s="14" t="s">
         <v>96</v>
       </c>
@@ -980,7 +1017,9 @@
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C6" t="s">
         <v>96</v>
       </c>
@@ -1004,7 +1043,9 @@
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C7" t="s">
         <v>96</v>
       </c>
@@ -1034,7 +1075,9 @@
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C8" t="s">
         <v>96</v>
       </c>
@@ -1134,6 +1177,9 @@
       <c r="C11" t="s">
         <v>96</v>
       </c>
+      <c r="D11" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="G11" s="14" t="s">
         <v>96</v>
       </c>
@@ -1148,14 +1194,26 @@
       <c r="B12" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -1164,7 +1222,12 @@
       <c r="B14" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -1173,7 +1236,12 @@
       <c r="B15" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -1182,7 +1250,12 @@
       <c r="B16" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
@@ -1191,7 +1264,12 @@
       <c r="B17" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
@@ -1200,7 +1278,12 @@
       <c r="B18" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
@@ -1209,7 +1292,12 @@
       <c r="B19" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
@@ -1218,14 +1306,23 @@
       <c r="B20" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="17"/>
+      <c r="B21" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="D21" s="14" t="s">
         <v>96</v>
       </c>
@@ -1249,7 +1346,9 @@
       <c r="B22" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="D22" s="14" t="s">
         <v>96</v>
       </c>
@@ -1273,7 +1372,9 @@
       <c r="B23" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="D23" s="14" t="s">
         <v>96</v>
       </c>
@@ -1297,7 +1398,9 @@
       <c r="B24" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="D24" s="14" t="s">
         <v>96</v>
       </c>
@@ -1318,7 +1421,9 @@
       <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C25" t="s">
         <v>96</v>
       </c>
@@ -1348,7 +1453,9 @@
       <c r="A26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C26" t="s">
         <v>96</v>
       </c>
@@ -1378,7 +1485,9 @@
       <c r="A27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C27" t="s">
         <v>96</v>
       </c>
@@ -1408,7 +1517,9 @@
       <c r="A28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="15"/>
+      <c r="B28" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C28" t="s">
         <v>96</v>
       </c>
@@ -1438,7 +1549,9 @@
       <c r="A29" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C29" t="s">
         <v>96</v>
       </c>
@@ -1468,7 +1581,9 @@
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C30" t="s">
         <v>96</v>
       </c>
@@ -1498,7 +1613,9 @@
       <c r="A31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C31" t="s">
         <v>96</v>
       </c>
@@ -1528,7 +1645,9 @@
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C32" t="s">
         <v>96</v>
       </c>
@@ -1558,7 +1677,9 @@
       <c r="A33" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="15"/>
+      <c r="B33" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C33" t="s">
         <v>96</v>
       </c>
@@ -1588,7 +1709,9 @@
       <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="15"/>
+      <c r="B34" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C34" t="s">
         <v>96</v>
       </c>
@@ -1638,7 +1761,9 @@
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C36" t="s">
         <v>96</v>
       </c>
@@ -1676,7 +1801,9 @@
       <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C39" t="s">
         <v>96</v>
       </c>
@@ -1706,7 +1833,9 @@
       <c r="A40" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="15"/>
+      <c r="B40" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C40" t="s">
         <v>96</v>
       </c>
@@ -1736,7 +1865,9 @@
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C41" t="s">
         <v>96</v>
       </c>
@@ -1850,7 +1981,9 @@
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="15"/>
+      <c r="B45" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C45" t="s">
         <v>96</v>
       </c>
@@ -1880,7 +2013,9 @@
       <c r="A46" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="15"/>
+      <c r="B46" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C46" t="s">
         <v>96</v>
       </c>
@@ -1910,7 +2045,9 @@
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="15"/>
+      <c r="B47" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C47" t="s">
         <v>96</v>
       </c>
@@ -1940,7 +2077,9 @@
       <c r="A48" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="15"/>
+      <c r="B48" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C48" t="s">
         <v>96</v>
       </c>
@@ -1970,7 +2109,9 @@
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="15"/>
+      <c r="B49" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C49" t="s">
         <v>96</v>
       </c>
@@ -1995,6 +2136,9 @@
       <c r="N49" s="14" t="s">
         <v>96</v>
       </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B50" s="20"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
@@ -2005,7 +2149,9 @@
       <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="15"/>
+      <c r="B52" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C52" t="s">
         <v>96</v>
       </c>
@@ -2035,7 +2181,9 @@
       <c r="A53" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="15"/>
+      <c r="B53" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C53" t="s">
         <v>96</v>
       </c>
@@ -2065,7 +2213,9 @@
       <c r="A54" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="15"/>
+      <c r="B54" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C54" t="s">
         <v>96</v>
       </c>
@@ -2095,7 +2245,9 @@
       <c r="A55" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="15"/>
+      <c r="B55" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C55" t="s">
         <v>96</v>
       </c>
@@ -2125,7 +2277,9 @@
       <c r="A56" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="15"/>
+      <c r="B56" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C56" t="s">
         <v>96</v>
       </c>
@@ -2155,7 +2309,9 @@
       <c r="A57" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="15"/>
+      <c r="B57" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C57" t="s">
         <v>96</v>
       </c>
@@ -2222,13 +2378,23 @@
       <c r="A61" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B61" s="15"/>
+      <c r="B61" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="15"/>
+      <c r="B62" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="F62" t="s">
         <v>96</v>
       </c>
@@ -2240,8 +2406,13 @@
       <c r="A63" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="15"/>
+      <c r="B63" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C63" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>96</v>
       </c>
       <c r="G63" s="14" t="s">
@@ -2271,6 +2442,9 @@
       <c r="C67" t="s">
         <v>96</v>
       </c>
+      <c r="D67" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E67" t="s">
         <v>96</v>
       </c>
@@ -2294,8 +2468,13 @@
       <c r="A68" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="15"/>
+      <c r="B68" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68" s="14" t="s">
         <v>96</v>
       </c>
       <c r="E68" t="s">
@@ -2327,6 +2506,9 @@
       <c r="C69" t="s">
         <v>96</v>
       </c>
+      <c r="D69" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E69" t="s">
         <v>96</v>
       </c>
@@ -2356,6 +2538,9 @@
       <c r="C70" t="s">
         <v>96</v>
       </c>
+      <c r="D70" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E70" t="s">
         <v>96</v>
       </c>
@@ -2385,6 +2570,9 @@
       <c r="C71" t="s">
         <v>96</v>
       </c>
+      <c r="D71" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E71" t="s">
         <v>96</v>
       </c>
@@ -2414,6 +2602,9 @@
       <c r="C72" t="s">
         <v>96</v>
       </c>
+      <c r="D72" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E72" t="s">
         <v>96</v>
       </c>
@@ -2443,6 +2634,9 @@
       <c r="C73" t="s">
         <v>96</v>
       </c>
+      <c r="D73" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E73" t="s">
         <v>96</v>
       </c>
@@ -2675,6 +2869,7 @@
       <c r="C85" t="s">
         <v>96</v>
       </c>
+      <c r="D85" s="15"/>
       <c r="E85" t="s">
         <v>96</v>
       </c>
@@ -2710,6 +2905,9 @@
       <c r="C86" t="s">
         <v>96</v>
       </c>
+      <c r="D86" t="s">
+        <v>96</v>
+      </c>
       <c r="E86" t="s">
         <v>96</v>
       </c>
@@ -2745,6 +2943,7 @@
       <c r="C87" t="s">
         <v>96</v>
       </c>
+      <c r="D87" s="15"/>
       <c r="E87" t="s">
         <v>96</v>
       </c>
@@ -2780,6 +2979,7 @@
       <c r="C88" t="s">
         <v>96</v>
       </c>
+      <c r="D88" s="15"/>
       <c r="E88" t="s">
         <v>96</v>
       </c>
@@ -2809,10 +3009,13 @@
       <c r="A89" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B89" s="15"/>
+      <c r="B89" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="C89" t="s">
         <v>96</v>
       </c>
+      <c r="D89" s="15"/>
       <c r="E89" t="s">
         <v>96</v>
       </c>
@@ -2848,6 +3051,7 @@
       <c r="C90" t="s">
         <v>96</v>
       </c>
+      <c r="D90" s="15"/>
       <c r="E90" t="s">
         <v>96</v>
       </c>
@@ -2940,6 +3144,9 @@
       <c r="C95" t="s">
         <v>96</v>
       </c>
+      <c r="D95" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E95" t="s">
         <v>96</v>
       </c>
@@ -2974,6 +3181,9 @@
       <c r="C98" t="s">
         <v>96</v>
       </c>
+      <c r="D98" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E98" t="s">
         <v>96</v>
       </c>
@@ -2997,6 +3207,9 @@
       <c r="C99" t="s">
         <v>96</v>
       </c>
+      <c r="D99" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E99" t="s">
         <v>96</v>
       </c>
@@ -3020,6 +3233,9 @@
       <c r="C100" t="s">
         <v>96</v>
       </c>
+      <c r="D100" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E100" t="s">
         <v>96</v>
       </c>
@@ -3043,6 +3259,9 @@
       <c r="C101" t="s">
         <v>96</v>
       </c>
+      <c r="D101" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="E101" t="s">
         <v>96</v>
       </c>
@@ -3077,6 +3296,7 @@
       <c r="C104" t="s">
         <v>96</v>
       </c>
+      <c r="D104" s="15"/>
       <c r="E104" t="s">
         <v>96</v>
       </c>
@@ -3105,8 +3325,15 @@
       <c r="A107" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B107" s="15"/>
-      <c r="C107" s="17"/>
+      <c r="B107" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C107" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>